<commit_message>
Updated BPEaCP to grow by GDP/capita
</commit_message>
<xml_diff>
--- a/InputData/io-model/BPEaCP/BAU Pop Employment and Compensation Projections.xlsx
+++ b/InputData/io-model/BPEaCP/BAU Pop Employment and Compensation Projections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\India\India_Model\InputData\io-model\BPEaCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E356E6F-8817-4F83-90DF-C171F2A3C8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F3052A-EF40-4B9A-83AF-488974C30BA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="1140" windowWidth="14505" windowHeight="14055" xr2:uid="{1123C965-C626-47FF-B97A-098977CD3CC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="7" xr2:uid="{1123C965-C626-47FF-B97A-098977CD3CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="BPEaCP-employedpop" sheetId="8" r:id="rId10"/>
     <sheet name="BPEaCP-employeecomp" sheetId="14" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="141">
   <si>
     <t>Sources:</t>
   </si>
@@ -399,9 +399,6 @@
     <t>GDP</t>
   </si>
   <si>
-    <t>Annual change in GDP</t>
-  </si>
-  <si>
     <t>2012 dollars per 2010 dollar</t>
   </si>
   <si>
@@ -462,7 +459,13 @@
     <t>2015 to 2012 dollars</t>
   </si>
   <si>
-    <t>We start with 2015 Total Employee Compensation and scale this value by forecasted real GDP growth</t>
+    <t>GDP/capita</t>
+  </si>
+  <si>
+    <t>Annual change in GDP/capita</t>
+  </si>
+  <si>
+    <t>We start with 2015 Total Employee Compensation and scale this value by forecasted real GDP growth/capita</t>
   </si>
 </sst>
 </file>
@@ -735,7 +738,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -795,6 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1393,7 +1397,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'EE Comp Projection'!$A$14</c:f>
+              <c:f>'EE Comp Projection'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1491,66 +1495,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'EE Comp Projection'!$B$14:$T$14</c:f>
+              <c:f>'EE Comp Projection'!$B$17:$T$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>648932705513.74646</c:v>
+                  <c:v>641400297495.39124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>707918846361.57983</c:v>
+                  <c:v>691713633583.62476</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>818344383532.20264</c:v>
+                  <c:v>790649865085.97888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>836980290061.51233</c:v>
+                  <c:v>799773367042.70142</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>886948415451.31848</c:v>
+                  <c:v>838426675251.40833</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>955425934734.17578</c:v>
+                  <c:v>893716391568.27246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1025215907034.9503</c:v>
+                  <c:v>949236651803.93542</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1096179983615.0687</c:v>
+                  <c:v>1004879967760.811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1168400674225.9873</c:v>
+                  <c:v>1060756822375.5968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1242245005003.4944</c:v>
+                  <c:v>1117232824968.7021</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1318060085936.4753</c:v>
+                  <c:v>1174645424660.4446</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1395943600983.551</c:v>
+                  <c:v>1233100663217.8279</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1476054879319.9473</c:v>
+                  <c:v>1292758282652.658</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1558453669386.3738</c:v>
+                  <c:v>1353697062165.1047</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1643170319597.1592</c:v>
+                  <c:v>1415974023742.0168</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1730209571892.0427</c:v>
+                  <c:v>1479623218445.8418</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1819567632719.2329</c:v>
+                  <c:v>1544667292592.5708</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1911171476206.7512</c:v>
+                  <c:v>1611073633592.0564</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2005029637846.1277</c:v>
+                  <c:v>1678889150994.0872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2945,13 +2949,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>638174</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>54769</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3279,7 +3283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D524350-AB87-478F-BE2E-F548EFE9AD6A}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -3378,12 +3382,12 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3393,12 +3397,12 @@
     </row>
     <row r="25" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3411,7 +3415,7 @@
     </row>
     <row r="29" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3421,12 +3425,12 @@
     </row>
     <row r="31" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -3434,7 +3438,7 @@
     </row>
     <row r="34" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3449,17 +3453,17 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3474,7 +3478,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3534,12 +3538,12 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3547,7 +3551,7 @@
         <v>0.9686815713640794</v>
       </c>
       <c r="B61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3555,7 +3559,7 @@
         <v>1.0529130131709286</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -3564,7 +3568,7 @@
         <v>1000000</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3958,132 +3962,132 @@
         <v>78</v>
       </c>
       <c r="B2" s="10">
-        <f>'EE Comp Projection'!F14</f>
-        <v>886948415451.31848</v>
+        <f>'EE Comp Projection'!F17</f>
+        <v>838426675251.40833</v>
       </c>
       <c r="C2" s="10">
-        <f>'EE Comp Projection'!G14</f>
-        <v>955425934734.17578</v>
+        <f>'EE Comp Projection'!G17</f>
+        <v>893716391568.27246</v>
       </c>
       <c r="D2" s="10">
-        <f>'EE Comp Projection'!H14</f>
-        <v>1025215907034.9503</v>
+        <f>'EE Comp Projection'!H17</f>
+        <v>949236651803.93542</v>
       </c>
       <c r="E2" s="10">
-        <f>'EE Comp Projection'!I14</f>
-        <v>1096179983615.0687</v>
+        <f>'EE Comp Projection'!I17</f>
+        <v>1004879967760.811</v>
       </c>
       <c r="F2" s="10">
-        <f>'EE Comp Projection'!J14</f>
-        <v>1168400674225.9873</v>
+        <f>'EE Comp Projection'!J17</f>
+        <v>1060756822375.5968</v>
       </c>
       <c r="G2" s="10">
-        <f>'EE Comp Projection'!K14</f>
-        <v>1242245005003.4944</v>
+        <f>'EE Comp Projection'!K17</f>
+        <v>1117232824968.7021</v>
       </c>
       <c r="H2" s="10">
-        <f>'EE Comp Projection'!L14</f>
-        <v>1318060085936.4753</v>
+        <f>'EE Comp Projection'!L17</f>
+        <v>1174645424660.4446</v>
       </c>
       <c r="I2" s="10">
-        <f>'EE Comp Projection'!M14</f>
-        <v>1395943600983.551</v>
+        <f>'EE Comp Projection'!M17</f>
+        <v>1233100663217.8279</v>
       </c>
       <c r="J2" s="10">
-        <f>'EE Comp Projection'!N14</f>
-        <v>1476054879319.9473</v>
+        <f>'EE Comp Projection'!N17</f>
+        <v>1292758282652.658</v>
       </c>
       <c r="K2" s="10">
-        <f>'EE Comp Projection'!O14</f>
-        <v>1558453669386.3738</v>
+        <f>'EE Comp Projection'!O17</f>
+        <v>1353697062165.1047</v>
       </c>
       <c r="L2" s="10">
-        <f>'EE Comp Projection'!P14</f>
-        <v>1643170319597.1592</v>
+        <f>'EE Comp Projection'!P17</f>
+        <v>1415974023742.0168</v>
       </c>
       <c r="M2" s="10">
-        <f>'EE Comp Projection'!Q14</f>
-        <v>1730209571892.0427</v>
+        <f>'EE Comp Projection'!Q17</f>
+        <v>1479623218445.8418</v>
       </c>
       <c r="N2" s="10">
-        <f>'EE Comp Projection'!R14</f>
-        <v>1819567632719.2329</v>
+        <f>'EE Comp Projection'!R17</f>
+        <v>1544667292592.5708</v>
       </c>
       <c r="O2" s="10">
-        <f>'EE Comp Projection'!S14</f>
-        <v>1911171476206.7512</v>
+        <f>'EE Comp Projection'!S17</f>
+        <v>1611073633592.0564</v>
       </c>
       <c r="P2" s="10">
-        <f>'EE Comp Projection'!T14</f>
-        <v>2005029637846.1277</v>
+        <f>'EE Comp Projection'!T17</f>
+        <v>1678889150994.0872</v>
       </c>
       <c r="Q2" s="10">
-        <f>'EE Comp Projection'!U14</f>
-        <v>2101112717610.9817</v>
+        <f>'EE Comp Projection'!U17</f>
+        <v>1748138532772.3655</v>
       </c>
       <c r="R2" s="10">
-        <f>'EE Comp Projection'!V14</f>
-        <v>2199362863836.4985</v>
+        <f>'EE Comp Projection'!V17</f>
+        <v>1818816724245.8384</v>
       </c>
       <c r="S2" s="10">
-        <f>'EE Comp Projection'!W14</f>
-        <v>2299726966797.603</v>
+        <f>'EE Comp Projection'!W17</f>
+        <v>1890923453403.4509</v>
       </c>
       <c r="T2" s="10">
-        <f>'EE Comp Projection'!X14</f>
-        <v>2402214510373.7729</v>
+        <f>'EE Comp Projection'!X17</f>
+        <v>1964499866591.8948</v>
       </c>
       <c r="U2" s="10">
-        <f>'EE Comp Projection'!Y14</f>
-        <v>2506849204263.7026</v>
+        <f>'EE Comp Projection'!Y17</f>
+        <v>2039581748138.4417</v>
       </c>
       <c r="V2" s="10">
-        <f>'EE Comp Projection'!Z14</f>
-        <v>2613631996855.3398</v>
+        <f>'EE Comp Projection'!Z17</f>
+        <v>2116175702311.8501</v>
       </c>
       <c r="W2" s="10">
-        <f>'EE Comp Projection'!AA14</f>
-        <v>2722543920389.729</v>
+        <f>'EE Comp Projection'!AA17</f>
+        <v>2194272644023.7856</v>
       </c>
       <c r="X2" s="10">
-        <f>'EE Comp Projection'!AB14</f>
-        <v>2833567903883.8105</v>
+        <f>'EE Comp Projection'!AB17</f>
+        <v>2273889902513.2534</v>
       </c>
       <c r="Y2" s="10">
-        <f>'EE Comp Projection'!AC14</f>
-        <v>2946761799002.3984</v>
+        <f>'EE Comp Projection'!AC17</f>
+        <v>2355105942434.8384</v>
       </c>
       <c r="Z2" s="10">
-        <f>'EE Comp Projection'!AD14</f>
-        <v>3062179663858.5156</v>
+        <f>'EE Comp Projection'!AD17</f>
+        <v>2437987535701.0747</v>
       </c>
       <c r="AA2" s="10">
-        <f>'EE Comp Projection'!AE14</f>
-        <v>3179828137167.7964</v>
+        <f>'EE Comp Projection'!AE17</f>
+        <v>2522557050588.6396</v>
       </c>
       <c r="AB2" s="10">
-        <f>'EE Comp Projection'!AF14</f>
-        <v>3299662644696.6958</v>
+        <f>'EE Comp Projection'!AF17</f>
+        <v>2608805142148.4937</v>
       </c>
       <c r="AC2" s="10">
-        <f>'EE Comp Projection'!AG14</f>
-        <v>3421631973496.0337</v>
+        <f>'EE Comp Projection'!AG17</f>
+        <v>2696716404456.8154</v>
       </c>
       <c r="AD2" s="10">
-        <f>'EE Comp Projection'!AH14</f>
-        <v>3545771213919.8784</v>
+        <f>'EE Comp Projection'!AH17</f>
+        <v>2786355670962.187</v>
       </c>
       <c r="AE2" s="10">
-        <f>'EE Comp Projection'!AI14</f>
-        <v>3672098385339.2373</v>
+        <f>'EE Comp Projection'!AI17</f>
+        <v>2877768559033.8711</v>
       </c>
       <c r="AF2" s="10">
-        <f>'EE Comp Projection'!AJ14</f>
-        <v>3800571758684.4077</v>
+        <f>'EE Comp Projection'!AJ17</f>
+        <v>2970967090346.1777</v>
       </c>
       <c r="AG2" s="10">
-        <f>'EE Comp Projection'!AK14</f>
-        <v>3931104082264.1948</v>
+        <f>'EE Comp Projection'!AK17</f>
+        <v>3065921038445.8809</v>
       </c>
       <c r="AH2" s="10"/>
     </row>
@@ -4453,7 +4457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F692D72D-FB12-4EFD-BBFA-B9A83A93CCFD}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8651,186 +8655,186 @@
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47"/>
-      <c r="Z3" s="47"/>
-      <c r="AA3" s="47"/>
-      <c r="AB3" s="47"/>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="47"/>
-      <c r="AI3" s="47"/>
-      <c r="AJ3" s="47"/>
-      <c r="AK3" s="47"/>
-      <c r="AL3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AJ3" s="48"/>
+      <c r="AK3" s="48"/>
+      <c r="AL3" s="49"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="41" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="42"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="42"/>
-      <c r="AC4" s="42"/>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="42"/>
-      <c r="AF4" s="42"/>
-      <c r="AG4" s="42"/>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="42"/>
-      <c r="AJ4" s="42"/>
-      <c r="AK4" s="42"/>
-      <c r="AL4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="44"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="41" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="42"/>
-      <c r="AE5" s="42"/>
-      <c r="AF5" s="42"/>
-      <c r="AG5" s="42"/>
-      <c r="AH5" s="42"/>
-      <c r="AI5" s="42"/>
-      <c r="AJ5" s="42"/>
-      <c r="AK5" s="42"/>
-      <c r="AL5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="43"/>
+      <c r="W5" s="43"/>
+      <c r="X5" s="43"/>
+      <c r="Y5" s="43"/>
+      <c r="Z5" s="43"/>
+      <c r="AA5" s="43"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
+      <c r="AD5" s="43"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="43"/>
+      <c r="AG5" s="43"/>
+      <c r="AH5" s="43"/>
+      <c r="AI5" s="43"/>
+      <c r="AJ5" s="43"/>
+      <c r="AK5" s="43"/>
+      <c r="AL5" s="44"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="V6" s="42"/>
-      <c r="W6" s="42"/>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="42"/>
-      <c r="Z6" s="42"/>
-      <c r="AA6" s="42"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
-      <c r="AD6" s="42"/>
-      <c r="AE6" s="42"/>
-      <c r="AF6" s="42"/>
-      <c r="AG6" s="42"/>
-      <c r="AH6" s="42"/>
-      <c r="AI6" s="42"/>
-      <c r="AJ6" s="42"/>
-      <c r="AK6" s="42"/>
-      <c r="AL6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="43"/>
+      <c r="W6" s="43"/>
+      <c r="X6" s="43"/>
+      <c r="Y6" s="43"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="43"/>
+      <c r="AB6" s="43"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="43"/>
+      <c r="AE6" s="43"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="43"/>
+      <c r="AH6" s="43"/>
+      <c r="AI6" s="43"/>
+      <c r="AJ6" s="43"/>
+      <c r="AK6" s="43"/>
+      <c r="AL6" s="44"/>
     </row>
     <row r="7" spans="1:38" ht="126" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="19" t="s">
         <v>33</v>
       </c>
@@ -9451,10 +9455,10 @@
         <v>105</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -10376,10 +10380,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10408,7 +10412,7 @@
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:53" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -10574,7 +10578,7 @@
         <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C4" s="10">
         <f t="array" ref="C4:BA4">TRANSPOSE(BGDP_calc!$C$45:$C$95)</f>
@@ -10733,316 +10737,602 @@
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27">
-        <f t="shared" ref="D5:T5" si="0">(D4-C4)/C4</f>
-        <v>3.6392531003638907E-2</v>
-      </c>
-      <c r="E5" s="27">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="array" ref="C5:BA5">TRANSPOSE('India Population Data'!B5:B55)</f>
+        <v>1053050912</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1071477855</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1089807112</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1108027848</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1126135777</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1144118674</v>
+      </c>
+      <c r="I5" s="10">
+        <v>1161977719</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1179681239</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1197146906</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1214270132</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1230980691</v>
+      </c>
+      <c r="N5" s="10">
+        <v>1247236029</v>
+      </c>
+      <c r="O5" s="10">
+        <v>1263065852</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1278562207</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>1293859294</v>
+      </c>
+      <c r="R5" s="10">
+        <v>1309053980</v>
+      </c>
+      <c r="S5" s="10">
+        <v>1324171354</v>
+      </c>
+      <c r="T5" s="10">
+        <v>1339180000</v>
+      </c>
+      <c r="U5" s="10">
+        <v>1354052000</v>
+      </c>
+      <c r="V5" s="10">
+        <v>1368738000</v>
+      </c>
+      <c r="W5">
+        <v>1383198000</v>
+      </c>
+      <c r="X5">
+        <v>1397423000</v>
+      </c>
+      <c r="Y5">
+        <v>1411415000</v>
+      </c>
+      <c r="Z5">
+        <v>1425158000</v>
+      </c>
+      <c r="AA5">
+        <v>1438635000</v>
+      </c>
+      <c r="AB5">
+        <v>1451829000</v>
+      </c>
+      <c r="AC5">
+        <v>1464726000</v>
+      </c>
+      <c r="AD5">
+        <v>1477312000</v>
+      </c>
+      <c r="AE5">
+        <v>1489565000</v>
+      </c>
+      <c r="AF5">
+        <v>1501462000</v>
+      </c>
+      <c r="AG5">
+        <v>1512985000</v>
+      </c>
+      <c r="AH5">
+        <v>1524124000</v>
+      </c>
+      <c r="AI5">
+        <v>1534869000</v>
+      </c>
+      <c r="AJ5">
+        <v>1545204000</v>
+      </c>
+      <c r="AK5">
+        <v>1555108000</v>
+      </c>
+      <c r="AL5">
+        <v>1564570000</v>
+      </c>
+      <c r="AM5">
+        <v>1573582000</v>
+      </c>
+      <c r="AN5">
+        <v>1582147000</v>
+      </c>
+      <c r="AO5">
+        <v>1590282000</v>
+      </c>
+      <c r="AP5">
+        <v>1598011000</v>
+      </c>
+      <c r="AQ5">
+        <v>1605356000</v>
+      </c>
+      <c r="AR5">
+        <v>1612320000</v>
+      </c>
+      <c r="AS5">
+        <v>1618906000</v>
+      </c>
+      <c r="AT5">
+        <v>1625123000</v>
+      </c>
+      <c r="AU5">
+        <v>1630984000</v>
+      </c>
+      <c r="AV5">
+        <v>1636496000</v>
+      </c>
+      <c r="AW5">
+        <v>1641667000</v>
+      </c>
+      <c r="AX5">
+        <v>1646498000</v>
+      </c>
+      <c r="AY5">
+        <v>1650994000</v>
+      </c>
+      <c r="AZ5">
+        <v>1655153000</v>
+      </c>
+      <c r="BA5">
+        <v>1658978000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="39">
+        <f>C4/C5</f>
+        <v>399.45298392758474</v>
+      </c>
+      <c r="D6" s="39">
+        <f t="shared" ref="D6:BA6" si="0">D4/D5</f>
+        <v>406.87041619880273</v>
+      </c>
+      <c r="E6" s="39">
         <f t="shared" si="0"/>
-        <v>6.0763168846529964E-2</v>
-      </c>
-      <c r="F5" s="27">
+        <v>424.33426947059542</v>
+      </c>
+      <c r="F6" s="39">
         <f t="shared" si="0"/>
-        <v>0.18014080486267542</v>
-      </c>
-      <c r="G5" s="27">
+        <v>492.53930821776783</v>
+      </c>
+      <c r="G6" s="39">
         <f t="shared" si="0"/>
-        <v>0.16693985298725042</v>
-      </c>
-      <c r="H5" s="27">
+        <v>565.52171747450063</v>
+      </c>
+      <c r="H6" s="39">
         <f t="shared" si="0"/>
-        <v>0.15685442243206574</v>
-      </c>
-      <c r="I5" s="27">
+        <v>643.94337689669408</v>
+      </c>
+      <c r="I6" s="39">
         <f t="shared" si="0"/>
-        <v>0.14612503978016722</v>
-      </c>
-      <c r="J5" s="27">
+        <v>726.69631032338248</v>
+      </c>
+      <c r="J6" s="39">
         <f t="shared" si="0"/>
-        <v>0.29404163256169646</v>
-      </c>
-      <c r="K5" s="27">
+        <v>926.26303317127349</v>
+      </c>
+      <c r="K6" s="39">
         <f t="shared" si="0"/>
-        <v>-1.4662069319678563E-2</v>
-      </c>
-      <c r="L5" s="27">
+        <v>899.36660704060921</v>
+      </c>
+      <c r="L6" s="39">
         <f t="shared" si="0"/>
-        <v>0.11926895285261774</v>
-      </c>
-      <c r="M5" s="27">
+        <v>992.43792128065422</v>
+      </c>
+      <c r="M6" s="39">
         <f t="shared" si="0"/>
-        <v>0.24870114367774579</v>
-      </c>
-      <c r="N5" s="27">
+        <v>1222.4354389021994</v>
+      </c>
+      <c r="N6" s="39">
         <f t="shared" si="0"/>
-        <v>8.7988613267859783E-2</v>
-      </c>
-      <c r="O5" s="27">
+        <v>1312.661884035901</v>
+      </c>
+      <c r="O6" s="39">
         <f t="shared" si="0"/>
-        <v>2.516361463081936E-3</v>
-      </c>
-      <c r="P5" s="27">
+        <v>1299.4722151889471</v>
+      </c>
+      <c r="P6" s="39">
         <f t="shared" si="0"/>
-        <v>1.5913580534270909E-2</v>
-      </c>
-      <c r="Q5" s="27">
+        <v>1304.151048169223</v>
+      </c>
+      <c r="Q6" s="39">
         <f t="shared" si="0"/>
-        <v>9.8240508260339601E-2</v>
-      </c>
-      <c r="R5" s="27">
+        <v>1415.3379979782824</v>
+      </c>
+      <c r="R6" s="39">
         <f t="shared" si="0"/>
-        <v>3.1611742002807461E-2</v>
-      </c>
-      <c r="S5" s="27">
+        <v>1443.1316034797367</v>
+      </c>
+      <c r="S6" s="39">
         <f t="shared" si="0"/>
-        <v>9.0897161364575277E-2</v>
-      </c>
-      <c r="T5" s="27">
+        <v>1556.3351140938692</v>
+      </c>
+      <c r="T6" s="39">
         <f t="shared" si="0"/>
-        <v>0.15598615256277742</v>
-      </c>
-      <c r="U5" s="27">
-        <f t="shared" ref="U5" si="1">(U4-T4)/T4</f>
-        <v>2.2772694362331928E-2</v>
-      </c>
-      <c r="V5" s="27">
-        <f t="shared" ref="V5" si="2">(V4-U4)/U4</f>
-        <v>5.970048038542683E-2</v>
-      </c>
-      <c r="W5" s="27">
-        <f t="shared" ref="W5" si="3">(W4-V4)/V4</f>
-        <v>7.7205751867782474E-2</v>
-      </c>
-      <c r="X5" s="27">
-        <f t="shared" ref="X5" si="4">(X4-W4)/W4</f>
-        <v>7.3045926181804846E-2</v>
-      </c>
-      <c r="Y5" s="27">
-        <f t="shared" ref="Y5" si="5">(Y4-X4)/X4</f>
-        <v>6.9218665154499273E-2</v>
-      </c>
-      <c r="Z5" s="27">
-        <f t="shared" ref="Z5" si="6">(Z4-Y4)/Y4</f>
-        <v>6.5883971328087487E-2</v>
-      </c>
-      <c r="AA5" s="27">
-        <f t="shared" ref="AA5" si="7">(AA4-Z4)/Z4</f>
-        <v>6.3201205208500727E-2</v>
-      </c>
-      <c r="AB5" s="27">
-        <f t="shared" ref="AB5" si="8">(AB4-AA4)/AA4</f>
-        <v>6.1030698958429545E-2</v>
-      </c>
-      <c r="AC5" s="27">
-        <f t="shared" ref="AC5" si="9">(AC4-AB4)/AB4</f>
-        <v>5.9089502730628407E-2</v>
-      </c>
-      <c r="AD5" s="27">
-        <f t="shared" ref="AD5" si="10">(AD4-AC4)/AC4</f>
-        <v>5.7388621058867682E-2</v>
-      </c>
-      <c r="AE5" s="27">
-        <f t="shared" ref="AE5" si="11">(AE4-AD4)/AD4</f>
-        <v>5.5823662941576806E-2</v>
-      </c>
-      <c r="AF5" s="27">
-        <f t="shared" ref="AF5" si="12">(AF4-AE4)/AE4</f>
-        <v>5.4359428114498801E-2</v>
-      </c>
-      <c r="AG5" s="27">
-        <f t="shared" ref="AG5" si="13">(AG4-AF4)/AF4</f>
-        <v>5.2970316744901998E-2</v>
-      </c>
-      <c r="AH5" s="27">
-        <f t="shared" ref="AH5" si="14">(AH4-AG4)/AG4</f>
-        <v>5.1645801918361801E-2</v>
-      </c>
-      <c r="AI5" s="27">
-        <f t="shared" ref="AI5" si="15">(AI4-AH4)/AH4</f>
-        <v>5.0343742018878312E-2</v>
-      </c>
-      <c r="AJ5" s="27">
-        <f t="shared" ref="AJ5" si="16">(AJ4-AI4)/AI4</f>
-        <v>4.9110277548545238E-2</v>
-      </c>
-      <c r="AK5" s="27">
-        <f t="shared" ref="AK5" si="17">(AK4-AJ4)/AJ4</f>
-        <v>4.7921027176471016E-2</v>
-      </c>
-      <c r="AL5" s="27">
-        <f t="shared" ref="AL5" si="18">(AL4-AK4)/AK4</f>
-        <v>4.6761006871268496E-2</v>
-      </c>
-      <c r="AM5" s="27">
-        <f t="shared" ref="AM5" si="19">(AM4-AL4)/AL4</f>
-        <v>4.5633262528600005E-2</v>
-      </c>
-      <c r="AN5" s="27">
-        <f t="shared" ref="AN5" si="20">(AN4-AM4)/AM4</f>
-        <v>4.4565091880835336E-2</v>
-      </c>
-      <c r="AO5" s="27">
-        <f t="shared" ref="AO5" si="21">(AO4-AN4)/AN4</f>
-        <v>4.355759797390004E-2</v>
-      </c>
-      <c r="AP5" s="27">
-        <f t="shared" ref="AP5" si="22">(AP4-AO4)/AO4</f>
-        <v>4.2596416413886819E-2</v>
-      </c>
-      <c r="AQ5" s="27">
-        <f t="shared" ref="AQ5" si="23">(AQ4-AP4)/AP4</f>
-        <v>4.1670718626581421E-2</v>
-      </c>
-      <c r="AR5" s="27">
-        <f t="shared" ref="AR5" si="24">(AR4-AQ4)/AQ4</f>
-        <v>4.077950135628617E-2</v>
-      </c>
-      <c r="AS5" s="27">
-        <f t="shared" ref="AS5" si="25">(AS4-AR4)/AR4</f>
-        <v>3.9947479276370788E-2</v>
-      </c>
-      <c r="AT5" s="27">
-        <f t="shared" ref="AT5" si="26">(AT4-AS4)/AS4</f>
-        <v>3.9167694143174753E-2</v>
-      </c>
-      <c r="AU5" s="27">
-        <f t="shared" ref="AU5" si="27">(AU4-AT4)/AT4</f>
-        <v>3.8419846718280783E-2</v>
-      </c>
-      <c r="AV5" s="27">
-        <f t="shared" ref="AV5" si="28">(AV4-AU4)/AU4</f>
-        <v>3.7685844127297093E-2</v>
-      </c>
-      <c r="AW5" s="27">
-        <f t="shared" ref="AW5" si="29">(AW4-AV4)/AV4</f>
-        <v>3.6964181473330401E-2</v>
-      </c>
-      <c r="AX5" s="27">
-        <f t="shared" ref="AX5" si="30">(AX4-AW4)/AW4</f>
-        <v>3.6280710896270475E-2</v>
-      </c>
-      <c r="AY5" s="27">
-        <f t="shared" ref="AY5" si="31">(AY4-AX4)/AX4</f>
-        <v>3.562755851912474E-2</v>
-      </c>
-      <c r="AZ5" s="27">
-        <f>(AZ4-AY4)/AY4</f>
-        <v>3.4986364705830594E-2</v>
-      </c>
-      <c r="BA5" s="27">
-        <f t="shared" ref="BA5" si="32">(BA4-AZ4)/AZ4</f>
-        <v>3.4345443756328808E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
-      <c r="AD6" s="26"/>
+        <v>1778.9386940544173</v>
+      </c>
+      <c r="U6" s="39">
+        <f t="shared" si="0"/>
+        <v>1799.466302257234</v>
+      </c>
+      <c r="V6" s="39">
+        <f t="shared" si="0"/>
+        <v>1886.435096741506</v>
+      </c>
+      <c r="W6" s="39">
+        <f t="shared" si="0"/>
+        <v>2010.8353149451298</v>
+      </c>
+      <c r="X6" s="39">
+        <f t="shared" si="0"/>
+        <v>2135.7542501130392</v>
+      </c>
+      <c r="Y6" s="39">
+        <f t="shared" si="0"/>
+        <v>2260.9500569957954</v>
+      </c>
+      <c r="Z6" s="39">
+        <f t="shared" si="0"/>
+        <v>2386.6713189168181</v>
+      </c>
+      <c r="AA6" s="39">
+        <f t="shared" si="0"/>
+        <v>2513.7406459791423</v>
+      </c>
+      <c r="AB6" s="39">
+        <f t="shared" si="0"/>
+        <v>2642.9172886726697</v>
+      </c>
+      <c r="AC6" s="39">
+        <f t="shared" si="0"/>
+        <v>2774.4398378210249</v>
+      </c>
+      <c r="AD6" s="39">
+        <f t="shared" si="0"/>
+        <v>2908.6677082023743</v>
+      </c>
+      <c r="AE6" s="39">
+        <f t="shared" si="0"/>
+        <v>3045.7781506753563</v>
+      </c>
+      <c r="AF6" s="39">
+        <f t="shared" si="0"/>
+        <v>3185.8994630153788</v>
+      </c>
+      <c r="AG6" s="39">
+        <f t="shared" si="0"/>
+        <v>3329.1082591007671</v>
+      </c>
+      <c r="AH6" s="39">
+        <f t="shared" si="0"/>
+        <v>3475.4554924693302</v>
+      </c>
+      <c r="AI6" s="39">
+        <f t="shared" si="0"/>
+        <v>3624.8677857626594</v>
+      </c>
+      <c r="AJ6" s="39">
+        <f t="shared" si="0"/>
+        <v>3777.4506840733729</v>
+      </c>
+      <c r="AK6" s="39">
+        <f t="shared" si="0"/>
+        <v>3933.2597346084408</v>
+      </c>
+      <c r="AL6" s="39">
+        <f t="shared" si="0"/>
+        <v>4092.2835644857473</v>
+      </c>
+      <c r="AM6" s="39">
+        <f t="shared" si="0"/>
+        <v>4254.5215616885043</v>
+      </c>
+      <c r="AN6" s="39">
+        <f t="shared" si="0"/>
+        <v>4420.0663042736751</v>
+      </c>
+      <c r="AO6" s="39">
+        <f t="shared" si="0"/>
+        <v>4588.9983059139186</v>
+      </c>
+      <c r="AP6" s="39">
+        <f t="shared" si="0"/>
+        <v>4761.3324260176259</v>
+      </c>
+      <c r="AQ6" s="39">
+        <f t="shared" si="0"/>
+        <v>4937.0482234061028</v>
+      </c>
+      <c r="AR6" s="39">
+        <f t="shared" si="0"/>
+        <v>5116.1846883519929</v>
+      </c>
+      <c r="AS6" s="39">
+        <f t="shared" si="0"/>
+        <v>5298.9183639957182</v>
+      </c>
+      <c r="AT6" s="39">
+        <f t="shared" si="0"/>
+        <v>5485.3994851556572</v>
+      </c>
+      <c r="AU6" s="39">
+        <f t="shared" si="0"/>
+        <v>5675.6783797894277</v>
+      </c>
+      <c r="AV6" s="39">
+        <f t="shared" si="0"/>
+        <v>5869.7340220394744</v>
+      </c>
+      <c r="AW6" s="39">
+        <f t="shared" si="0"/>
+        <v>6067.5317490351463</v>
+      </c>
+      <c r="AX6" s="39">
+        <f t="shared" si="0"/>
+        <v>6269.217434108552</v>
+      </c>
+      <c r="AY6" s="39">
+        <f t="shared" si="0"/>
+        <v>6474.8937149845387</v>
+      </c>
+      <c r="AZ6" s="39">
+        <f t="shared" si="0"/>
+        <v>6684.5876400729539</v>
+      </c>
+      <c r="BA6" s="39">
+        <f t="shared" si="0"/>
+        <v>6898.2312007525315</v>
+      </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="26"/>
+      <c r="A7" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <f>SUM('OECD VAL'!C9:AL9)*10^6</f>
-        <v>649385143000.00012</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
-      <c r="AD8" s="26"/>
+      <c r="A8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27">
+        <f>(D6-C6)/C6</f>
+        <v>1.8568974496790007E-2</v>
+      </c>
+      <c r="E8" s="27">
+        <f t="shared" ref="E8:BA8" si="1">(E6-D6)/D6</f>
+        <v>4.2922396361350583E-2</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.16073422217881633</v>
+      </c>
+      <c r="G8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.14817580655809279</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.13867134894908695</v>
+      </c>
+      <c r="I8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.12850964292154557</v>
+      </c>
+      <c r="J8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.27462190190436375</v>
+      </c>
+      <c r="K8" s="27">
+        <f t="shared" si="1"/>
+        <v>-2.9037568344467132E-2</v>
+      </c>
+      <c r="L8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.10348540129402709</v>
+      </c>
+      <c r="M8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.23175002958850416</v>
+      </c>
+      <c r="N8" s="27">
+        <f t="shared" si="1"/>
+        <v>7.3808760988415836E-2</v>
+      </c>
+      <c r="O8" s="27">
+        <f t="shared" si="1"/>
+        <v>-1.0048032175963775E-2</v>
+      </c>
+      <c r="P8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.6005640794679401E-3</v>
+      </c>
+      <c r="Q8" s="27">
+        <f t="shared" si="1"/>
+        <v>8.5256190197557563E-2</v>
+      </c>
+      <c r="R8" s="27">
+        <f t="shared" si="1"/>
+        <v>1.9637433278238584E-2</v>
+      </c>
+      <c r="S8" s="27">
+        <f t="shared" si="1"/>
+        <v>7.8442957205823532E-2</v>
+      </c>
+      <c r="T8" s="27">
+        <f t="shared" si="1"/>
+        <v>0.14303062235420461</v>
+      </c>
+      <c r="U8" s="27">
+        <f t="shared" si="1"/>
+        <v>1.1539244309781033E-2</v>
+      </c>
+      <c r="V8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.8330326817000731E-2</v>
+      </c>
+      <c r="W8" s="27">
+        <f t="shared" si="1"/>
+        <v>6.5944605472249701E-2</v>
+      </c>
+      <c r="X8" s="27">
+        <f t="shared" si="1"/>
+        <v>6.2122906952883986E-2</v>
+      </c>
+      <c r="Y8" s="27">
+        <f t="shared" si="1"/>
+        <v>5.8619013342068704E-2</v>
+      </c>
+      <c r="Z8" s="27">
+        <f t="shared" si="1"/>
+        <v>5.5605501559850015E-2</v>
+      </c>
+      <c r="AA8" s="27">
+        <f t="shared" si="1"/>
+        <v>5.3241234373233318E-2</v>
+      </c>
+      <c r="AB8" s="27">
+        <f t="shared" si="1"/>
+        <v>5.1388214174024699E-2</v>
+      </c>
+      <c r="AC8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.9764156340438744E-2</v>
+      </c>
+      <c r="AD8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.8380169773934854E-2</v>
+      </c>
+      <c r="AE8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.7138572098261257E-2</v>
+      </c>
+      <c r="AF8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.6005094727254746E-2</v>
+      </c>
+      <c r="AG8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.4950820874254616E-2</v>
+      </c>
+      <c r="AH8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.3959890150311098E-2</v>
+      </c>
+      <c r="AI8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.2990708301998977E-2</v>
+      </c>
+      <c r="AJ8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.2093369283704954E-2</v>
+      </c>
+      <c r="AK8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.1247143527775421E-2</v>
+      </c>
+      <c r="AL8" s="27">
+        <f t="shared" si="1"/>
+        <v>4.0430543774688577E-2</v>
+      </c>
+      <c r="AM8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.9644857118581539E-2</v>
+      </c>
+      <c r="AN8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.8910307583320959E-2</v>
+      </c>
+      <c r="AO8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.8219336546355981E-2</v>
+      </c>
+      <c r="AP8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.7553755441926739E-2</v>
+      </c>
+      <c r="AQ8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.6904753053641624E-2</v>
+      </c>
+      <c r="AR8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.6284122990053083E-2</v>
+      </c>
+      <c r="AS8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.571678638962246E-2</v>
+      </c>
+      <c r="AT8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.5192299324143667E-2</v>
+      </c>
+      <c r="AU8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.468824743734613E-2</v>
+      </c>
+      <c r="AV8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.4190739725679514E-2</v>
+      </c>
+      <c r="AW8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.3697902878220339E-2</v>
+      </c>
+      <c r="AX8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.3240153231250513E-2</v>
+      </c>
+      <c r="AY8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.2807329309871479E-2</v>
+      </c>
+      <c r="AZ8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.2385693776429178E-2</v>
+      </c>
+      <c r="BA8" s="27">
+        <f t="shared" si="1"/>
+        <v>3.1960619290683119E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <f>A8*About!$A$61</f>
-        <v>629047420741.72754</v>
-      </c>
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
@@ -11072,6 +11362,10 @@
       <c r="AD9" s="26"/>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="9"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
@@ -11101,421 +11395,527 @@
       <c r="AD10" s="26"/>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="10">
+        <f>SUM('OECD VAL'!C9:AL9)*10^6</f>
+        <v>649385143000.00012</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="26"/>
+      <c r="AD11" s="26"/>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <f>A11*About!$A$61</f>
+        <v>629047420741.72754</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>2015</v>
       </c>
-      <c r="C12">
+      <c r="C15">
         <v>2016</v>
       </c>
-      <c r="D12">
+      <c r="D15">
         <v>2017</v>
       </c>
-      <c r="E12">
+      <c r="E15">
         <v>2018</v>
       </c>
-      <c r="F12">
+      <c r="F15">
         <v>2019</v>
       </c>
-      <c r="G12">
+      <c r="G15">
         <v>2020</v>
       </c>
-      <c r="H12">
+      <c r="H15">
         <v>2021</v>
       </c>
-      <c r="I12">
+      <c r="I15">
         <v>2022</v>
       </c>
-      <c r="J12">
+      <c r="J15">
         <v>2023</v>
       </c>
-      <c r="K12">
+      <c r="K15">
         <v>2024</v>
       </c>
-      <c r="L12">
+      <c r="L15">
         <v>2025</v>
       </c>
-      <c r="M12">
+      <c r="M15">
         <v>2026</v>
       </c>
-      <c r="N12">
+      <c r="N15">
         <v>2027</v>
       </c>
-      <c r="O12">
+      <c r="O15">
         <v>2028</v>
       </c>
-      <c r="P12">
+      <c r="P15">
         <v>2029</v>
       </c>
-      <c r="Q12">
+      <c r="Q15">
         <v>2030</v>
       </c>
-      <c r="R12">
+      <c r="R15">
         <v>2031</v>
       </c>
-      <c r="S12">
+      <c r="S15">
         <v>2032</v>
       </c>
-      <c r="T12">
+      <c r="T15">
         <v>2033</v>
       </c>
-      <c r="U12">
+      <c r="U15">
         <v>2034</v>
       </c>
-      <c r="V12">
+      <c r="V15">
         <v>2035</v>
       </c>
-      <c r="W12">
+      <c r="W15">
         <v>2036</v>
       </c>
-      <c r="X12">
+      <c r="X15">
         <v>2037</v>
       </c>
-      <c r="Y12">
+      <c r="Y15">
         <v>2038</v>
       </c>
-      <c r="Z12">
+      <c r="Z15">
         <v>2039</v>
       </c>
-      <c r="AA12">
+      <c r="AA15">
         <v>2040</v>
       </c>
-      <c r="AB12">
+      <c r="AB15">
         <v>2041</v>
       </c>
-      <c r="AC12">
+      <c r="AC15">
         <v>2042</v>
       </c>
-      <c r="AD12">
+      <c r="AD15">
         <v>2043</v>
       </c>
-      <c r="AE12">
+      <c r="AE15">
         <v>2044</v>
       </c>
-      <c r="AF12">
+      <c r="AF15">
         <v>2045</v>
       </c>
-      <c r="AG12">
+      <c r="AG15">
         <v>2046</v>
       </c>
-      <c r="AH12">
+      <c r="AH15">
         <v>2047</v>
       </c>
-      <c r="AI12">
+      <c r="AI15">
         <v>2048</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ15">
         <v>2049</v>
       </c>
-      <c r="AK12">
+      <c r="AK15">
         <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="11">
-        <f>R5</f>
-        <v>3.1611742002807461E-2</v>
-      </c>
-      <c r="C13" s="11">
-        <f t="shared" ref="C13:E13" si="33">S5</f>
-        <v>9.0897161364575277E-2</v>
-      </c>
-      <c r="D13" s="11">
-        <f t="shared" si="33"/>
-        <v>0.15598615256277742</v>
-      </c>
-      <c r="E13" s="11">
-        <f t="shared" si="33"/>
-        <v>2.2772694362331928E-2</v>
-      </c>
-      <c r="F13" s="11">
-        <f t="shared" ref="F13:AK13" si="34">V5</f>
-        <v>5.970048038542683E-2</v>
-      </c>
-      <c r="G13" s="11">
-        <f t="shared" si="34"/>
-        <v>7.7205751867782474E-2</v>
-      </c>
-      <c r="H13" s="11">
-        <f t="shared" si="34"/>
-        <v>7.3045926181804846E-2</v>
-      </c>
-      <c r="I13" s="11">
-        <f t="shared" si="34"/>
-        <v>6.9218665154499273E-2</v>
-      </c>
-      <c r="J13" s="11">
-        <f t="shared" si="34"/>
-        <v>6.5883971328087487E-2</v>
-      </c>
-      <c r="K13" s="11">
-        <f t="shared" si="34"/>
-        <v>6.3201205208500727E-2</v>
-      </c>
-      <c r="L13" s="11">
-        <f t="shared" si="34"/>
-        <v>6.1030698958429545E-2</v>
-      </c>
-      <c r="M13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.9089502730628407E-2</v>
-      </c>
-      <c r="N13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.7388621058867682E-2</v>
-      </c>
-      <c r="O13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.5823662941576806E-2</v>
-      </c>
-      <c r="P13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.4359428114498801E-2</v>
-      </c>
-      <c r="Q13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.2970316744901998E-2</v>
-      </c>
-      <c r="R13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.1645801918361801E-2</v>
-      </c>
-      <c r="S13" s="11">
-        <f t="shared" si="34"/>
-        <v>5.0343742018878312E-2</v>
-      </c>
-      <c r="T13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.9110277548545238E-2</v>
-      </c>
-      <c r="U13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.7921027176471016E-2</v>
-      </c>
-      <c r="V13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.6761006871268496E-2</v>
-      </c>
-      <c r="W13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.5633262528600005E-2</v>
-      </c>
-      <c r="X13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.4565091880835336E-2</v>
-      </c>
-      <c r="Y13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.355759797390004E-2</v>
-      </c>
-      <c r="Z13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.2596416413886819E-2</v>
-      </c>
-      <c r="AA13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.1670718626581421E-2</v>
-      </c>
-      <c r="AB13" s="11">
-        <f t="shared" si="34"/>
-        <v>4.077950135628617E-2</v>
-      </c>
-      <c r="AC13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.9947479276370788E-2</v>
-      </c>
-      <c r="AD13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.9167694143174753E-2</v>
-      </c>
-      <c r="AE13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.8419846718280783E-2</v>
-      </c>
-      <c r="AF13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.7685844127297093E-2</v>
-      </c>
-      <c r="AG13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.6964181473330401E-2</v>
-      </c>
-      <c r="AH13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.6280710896270475E-2</v>
-      </c>
-      <c r="AI13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.562755851912474E-2</v>
-      </c>
-      <c r="AJ13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.4986364705830594E-2</v>
-      </c>
-      <c r="AK13" s="11">
-        <f t="shared" si="34"/>
-        <v>3.4345443756328808E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="11">
+        <f>R8</f>
+        <v>1.9637433278238584E-2</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" ref="C16:E16" si="2">S8</f>
+        <v>7.8442957205823532E-2</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="2"/>
+        <v>0.14303062235420461</v>
+      </c>
+      <c r="E16" s="11">
+        <f t="shared" si="2"/>
+        <v>1.1539244309781033E-2</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" ref="F16:AK16" si="3">V8</f>
+        <v>4.8330326817000731E-2</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="3"/>
+        <v>6.5944605472249701E-2</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="3"/>
+        <v>6.2122906952883986E-2</v>
+      </c>
+      <c r="I16" s="11">
+        <f t="shared" si="3"/>
+        <v>5.8619013342068704E-2</v>
+      </c>
+      <c r="J16" s="11">
+        <f t="shared" si="3"/>
+        <v>5.5605501559850015E-2</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="3"/>
+        <v>5.3241234373233318E-2</v>
+      </c>
+      <c r="L16" s="11">
+        <f t="shared" si="3"/>
+        <v>5.1388214174024699E-2</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.9764156340438744E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.8380169773934854E-2</v>
+      </c>
+      <c r="O16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.7138572098261257E-2</v>
+      </c>
+      <c r="P16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.6005094727254746E-2</v>
+      </c>
+      <c r="Q16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.4950820874254616E-2</v>
+      </c>
+      <c r="R16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.3959890150311098E-2</v>
+      </c>
+      <c r="S16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2990708301998977E-2</v>
+      </c>
+      <c r="T16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.2093369283704954E-2</v>
+      </c>
+      <c r="U16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.1247143527775421E-2</v>
+      </c>
+      <c r="V16" s="11">
+        <f t="shared" si="3"/>
+        <v>4.0430543774688577E-2</v>
+      </c>
+      <c r="W16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.9644857118581539E-2</v>
+      </c>
+      <c r="X16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.8910307583320959E-2</v>
+      </c>
+      <c r="Y16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.8219336546355981E-2</v>
+      </c>
+      <c r="Z16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.7553755441926739E-2</v>
+      </c>
+      <c r="AA16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.6904753053641624E-2</v>
+      </c>
+      <c r="AB16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.6284122990053083E-2</v>
+      </c>
+      <c r="AC16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.571678638962246E-2</v>
+      </c>
+      <c r="AD16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.5192299324143667E-2</v>
+      </c>
+      <c r="AE16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.468824743734613E-2</v>
+      </c>
+      <c r="AF16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.4190739725679514E-2</v>
+      </c>
+      <c r="AG16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.3697902878220339E-2</v>
+      </c>
+      <c r="AH16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.3240153231250513E-2</v>
+      </c>
+      <c r="AI16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.2807329309871479E-2</v>
+      </c>
+      <c r="AJ16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.2385693776429178E-2</v>
+      </c>
+      <c r="AK16" s="11">
+        <f t="shared" si="3"/>
+        <v>3.1960619290683119E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="13">
-        <f>A9*(1+B13)</f>
-        <v>648932705513.74646</v>
-      </c>
-      <c r="C14" s="13">
-        <f>B14*(1+C13)</f>
-        <v>707918846361.57983</v>
-      </c>
-      <c r="D14" s="13">
-        <f t="shared" ref="D14:AK14" si="35">C14*(1+D13)</f>
-        <v>818344383532.20264</v>
-      </c>
-      <c r="E14" s="13">
-        <f t="shared" si="35"/>
-        <v>836980290061.51233</v>
-      </c>
-      <c r="F14" s="13">
-        <f>E14*(1+F13)</f>
-        <v>886948415451.31848</v>
-      </c>
-      <c r="G14" s="13">
-        <f t="shared" si="35"/>
-        <v>955425934734.17578</v>
-      </c>
-      <c r="H14" s="13">
-        <f t="shared" si="35"/>
-        <v>1025215907034.9503</v>
-      </c>
-      <c r="I14" s="13">
-        <f t="shared" si="35"/>
-        <v>1096179983615.0687</v>
-      </c>
-      <c r="J14" s="13">
-        <f t="shared" si="35"/>
-        <v>1168400674225.9873</v>
-      </c>
-      <c r="K14" s="13">
-        <f t="shared" si="35"/>
-        <v>1242245005003.4944</v>
-      </c>
-      <c r="L14" s="13">
-        <f t="shared" si="35"/>
-        <v>1318060085936.4753</v>
-      </c>
-      <c r="M14" s="13">
-        <f t="shared" si="35"/>
-        <v>1395943600983.551</v>
-      </c>
-      <c r="N14" s="13">
-        <f t="shared" si="35"/>
-        <v>1476054879319.9473</v>
-      </c>
-      <c r="O14" s="13">
-        <f t="shared" si="35"/>
-        <v>1558453669386.3738</v>
-      </c>
-      <c r="P14" s="13">
-        <f t="shared" si="35"/>
-        <v>1643170319597.1592</v>
-      </c>
-      <c r="Q14" s="13">
-        <f t="shared" si="35"/>
-        <v>1730209571892.0427</v>
-      </c>
-      <c r="R14" s="13">
-        <f t="shared" si="35"/>
-        <v>1819567632719.2329</v>
-      </c>
-      <c r="S14" s="13">
-        <f t="shared" si="35"/>
-        <v>1911171476206.7512</v>
-      </c>
-      <c r="T14" s="13">
-        <f t="shared" si="35"/>
-        <v>2005029637846.1277</v>
-      </c>
-      <c r="U14" s="13">
-        <f t="shared" si="35"/>
-        <v>2101112717610.9817</v>
-      </c>
-      <c r="V14" s="13">
-        <f t="shared" si="35"/>
-        <v>2199362863836.4985</v>
-      </c>
-      <c r="W14" s="13">
-        <f t="shared" si="35"/>
-        <v>2299726966797.603</v>
-      </c>
-      <c r="X14" s="13">
-        <f t="shared" si="35"/>
-        <v>2402214510373.7729</v>
-      </c>
-      <c r="Y14" s="13">
-        <f t="shared" si="35"/>
-        <v>2506849204263.7026</v>
-      </c>
-      <c r="Z14" s="13">
-        <f t="shared" si="35"/>
-        <v>2613631996855.3398</v>
-      </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="35"/>
-        <v>2722543920389.729</v>
-      </c>
-      <c r="AB14" s="13">
-        <f t="shared" si="35"/>
-        <v>2833567903883.8105</v>
-      </c>
-      <c r="AC14" s="13">
-        <f t="shared" si="35"/>
-        <v>2946761799002.3984</v>
-      </c>
-      <c r="AD14" s="13">
-        <f t="shared" si="35"/>
-        <v>3062179663858.5156</v>
-      </c>
-      <c r="AE14" s="13">
-        <f t="shared" si="35"/>
-        <v>3179828137167.7964</v>
-      </c>
-      <c r="AF14" s="13">
-        <f t="shared" si="35"/>
-        <v>3299662644696.6958</v>
-      </c>
-      <c r="AG14" s="13">
-        <f t="shared" si="35"/>
-        <v>3421631973496.0337</v>
-      </c>
-      <c r="AH14" s="13">
-        <f t="shared" si="35"/>
-        <v>3545771213919.8784</v>
-      </c>
-      <c r="AI14" s="13">
-        <f t="shared" si="35"/>
-        <v>3672098385339.2373</v>
-      </c>
-      <c r="AJ14" s="13">
-        <f t="shared" si="35"/>
-        <v>3800571758684.4077</v>
-      </c>
-      <c r="AK14" s="13">
-        <f t="shared" si="35"/>
-        <v>3931104082264.1948</v>
-      </c>
+      <c r="B17" s="13">
+        <f>A12*(1+B16)</f>
+        <v>641400297495.39124</v>
+      </c>
+      <c r="C17" s="13">
+        <f>B17*(1+C16)</f>
+        <v>691713633583.62476</v>
+      </c>
+      <c r="D17" s="13">
+        <f t="shared" ref="D17:AK17" si="4">C17*(1+D16)</f>
+        <v>790649865085.97888</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="4"/>
+        <v>799773367042.70142</v>
+      </c>
+      <c r="F17" s="13">
+        <f>E17*(1+F16)</f>
+        <v>838426675251.40833</v>
+      </c>
+      <c r="G17" s="13">
+        <f t="shared" si="4"/>
+        <v>893716391568.27246</v>
+      </c>
+      <c r="H17" s="13">
+        <f t="shared" si="4"/>
+        <v>949236651803.93542</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" si="4"/>
+        <v>1004879967760.811</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" si="4"/>
+        <v>1060756822375.5968</v>
+      </c>
+      <c r="K17" s="13">
+        <f t="shared" si="4"/>
+        <v>1117232824968.7021</v>
+      </c>
+      <c r="L17" s="13">
+        <f>K17*(1+L16)</f>
+        <v>1174645424660.4446</v>
+      </c>
+      <c r="M17" s="13">
+        <f t="shared" si="4"/>
+        <v>1233100663217.8279</v>
+      </c>
+      <c r="N17" s="13">
+        <f t="shared" si="4"/>
+        <v>1292758282652.658</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="4"/>
+        <v>1353697062165.1047</v>
+      </c>
+      <c r="P17" s="13">
+        <f t="shared" si="4"/>
+        <v>1415974023742.0168</v>
+      </c>
+      <c r="Q17" s="13">
+        <f t="shared" si="4"/>
+        <v>1479623218445.8418</v>
+      </c>
+      <c r="R17" s="13">
+        <f t="shared" si="4"/>
+        <v>1544667292592.5708</v>
+      </c>
+      <c r="S17" s="13">
+        <f t="shared" si="4"/>
+        <v>1611073633592.0564</v>
+      </c>
+      <c r="T17" s="13">
+        <f t="shared" si="4"/>
+        <v>1678889150994.0872</v>
+      </c>
+      <c r="U17" s="13">
+        <f t="shared" si="4"/>
+        <v>1748138532772.3655</v>
+      </c>
+      <c r="V17" s="13">
+        <f t="shared" si="4"/>
+        <v>1818816724245.8384</v>
+      </c>
+      <c r="W17" s="13">
+        <f t="shared" si="4"/>
+        <v>1890923453403.4509</v>
+      </c>
+      <c r="X17" s="13">
+        <f t="shared" si="4"/>
+        <v>1964499866591.8948</v>
+      </c>
+      <c r="Y17" s="13">
+        <f t="shared" si="4"/>
+        <v>2039581748138.4417</v>
+      </c>
+      <c r="Z17" s="13">
+        <f t="shared" si="4"/>
+        <v>2116175702311.8501</v>
+      </c>
+      <c r="AA17" s="13">
+        <f t="shared" si="4"/>
+        <v>2194272644023.7856</v>
+      </c>
+      <c r="AB17" s="13">
+        <f t="shared" si="4"/>
+        <v>2273889902513.2534</v>
+      </c>
+      <c r="AC17" s="13">
+        <f t="shared" si="4"/>
+        <v>2355105942434.8384</v>
+      </c>
+      <c r="AD17" s="13">
+        <f t="shared" si="4"/>
+        <v>2437987535701.0747</v>
+      </c>
+      <c r="AE17" s="13">
+        <f t="shared" si="4"/>
+        <v>2522557050588.6396</v>
+      </c>
+      <c r="AF17" s="13">
+        <f t="shared" si="4"/>
+        <v>2608805142148.4937</v>
+      </c>
+      <c r="AG17" s="13">
+        <f t="shared" si="4"/>
+        <v>2696716404456.8154</v>
+      </c>
+      <c r="AH17" s="13">
+        <f t="shared" si="4"/>
+        <v>2786355670962.187</v>
+      </c>
+      <c r="AI17" s="13">
+        <f t="shared" si="4"/>
+        <v>2877768559033.8711</v>
+      </c>
+      <c r="AJ17" s="13">
+        <f t="shared" si="4"/>
+        <v>2970967090346.1777</v>
+      </c>
+      <c r="AK17" s="13">
+        <f t="shared" si="4"/>
+        <v>3065921038445.8809</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="AK19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>